<commit_message>
[Tejas Tonpe] Add: performed summarization & translation on email body using prompts.
</commit_message>
<xml_diff>
--- a/SummarizedEmails.xlsx
+++ b/SummarizedEmails.xlsx
@@ -493,14 +493,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>```
-Kaustubh Kale applies for the Software Developer position, highlighting his 5+ years of experience in Java, Python, and C++, and his ability to design and implement software solutions. He's eager to discuss how his skills can benefit the company. 
-```</t>
+          <t>Kaustubh Kale, a software developer with 5+ years of experience in Java, Python, and C++, expresses interest in the advertised position. He highlights his skills, experience, and desire to contribute to the team, attaching his resume and cover letter for review.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Kaustubh Kale solicita el puesto de Desarrollador de Software, destacando sus más de 5 años de experiencia en Java, Python y C++, y su capacidad para diseñar e implementar soluciones de software. Está ansioso por discutir cómo sus habilidades pueden beneficiar a la empresa.</t>
+          <t>Kaustubh Kale, un desarrollador de software con más de 5 años de experiencia en Java, Python y C++, expresa su interés en el puesto anunciado. Destaca sus habilidades, experiencia y deseo de contribuir al equipo, adjuntando su currículum vitae y carta de presentación para su revisión.</t>
         </is>
       </c>
     </row>
@@ -531,14 +529,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>```
-Tejas requests a meeting with Kaustubh this week to discuss the project timeline, milestones, and deliverables to ensure the project stays on track. 
-```</t>
+          <t>Tejas requests a meeting this week with Kaustubh to discuss the project timeline, ensuring alignment on milestones and deliverables before the deadline.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Tejas solicita una reunión con Kaustubh esta semana para discutir el cronograma del proyecto, los hitos y los entregables para garantizar que el proyecto se mantenga en camino.</t>
+          <t>Tejas solicita una reunión esta semana con Kaustubh para discutir el cronograma del proyecto, asegurando la alineación en los hitos y entregables antes de la fecha límite.</t>
         </is>
       </c>
     </row>
@@ -570,14 +566,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>```
-Niraj is following up on the meeting regarding the client's marketing campaign, requesting branding guidelines, images, and copy by Friday to begin design. 
-```</t>
+          <t>The email requests branding guidelines, high-resolution images, and copy for the marketing campaign by Friday to begin the design phase and meet deadlines.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Niraj está haciendo seguimiento de la reunión sobre la campaña de marketing del cliente, solicitando las pautas de marca, imágenes y copia para el viernes para comenzar el diseño.</t>
+          <t>El correo electrónico solicita las directrices de marca, imágenes de alta resolución y el texto para la campaña de marketing para el viernes para comenzar la fase de diseño y cumplir con las fechas límite.</t>
         </is>
       </c>
     </row>
@@ -609,14 +603,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>```
-Saloni Goyal inquires about international student admission requirements, including documentation, English proficiency tests, deadlines, and scholarships. 
-```</t>
+          <t>Saloni Goyal inquires about international student admission requirements, including documentation, English proficiency tests, deadlines, and scholarship opportunities.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Saloni Goyal pregunta por los requisitos de admisión para estudiantes internacionales, incluyendo la documentación, las pruebas de dominio del inglés, las fechas límite y las becas.</t>
+          <t>Saloni Goyal consulta sobre los requisitos de admisión para estudiantes internacionales, incluyendo la documentación, las pruebas de dominio del inglés, las fechas límite y las oportunidades de becas.</t>
         </is>
       </c>
     </row>
@@ -648,14 +640,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>```
-Niraj wadhe reports a defective blender (Order #12345) and requests instructions for return and refund/replacement, emphasizing urgency due to need for a functional blender. 
-```</t>
+          <t>Customer Niraj Wadhe reports a defective blender (Order #12345) and requests instructions for return and replacement, emphasizing the urgent need for a functional blender.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Niraj Wadhe reporta una licuadora defectuosa (orden #12345) y solicita instrucciones para la devolución y el reembolso/reemplazo, enfatizando la urgencia debido a la necesidad de una licuadora funcional.</t>
+          <t>El cliente Niraj Wadhe reporta una licuadora defectuosa (Orden #12345) y solicita instrucciones para la devolución y reemplazo, enfatizando la necesidad urgente de una licuadora funcional.</t>
         </is>
       </c>
     </row>
@@ -686,14 +676,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>```
-Tejas expresses gratitude to Kaustubh for his valuable contributions to the project, highlighting his expertise and dedication, and offering future assistance. 
-```</t>
+          <t>Tejas expresses gratitude to Kaustubh for his exceptional contributions to the project, highlighting his expertise, dedication, and willingness to go the extra mile.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Tejas expresa su agradecimiento a Kaustubh por sus valiosas contribuciones al proyecto, destacando su experiencia y dedicación, y ofreciendo su ayuda en el futuro.</t>
+          <t>Tejas expresa su agradecimiento a Kaustubh por sus excepcionales contribuciones al proyecto, destacando su experiencia, dedicación y disposición a esforzarse más allá de lo esperado.</t>
         </is>
       </c>
     </row>
@@ -724,16 +712,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>```
-You are invited to the Annual Gala on July 20th at 7:00 PM with dinner, entertainment, and an auction. RSVP by July 10th. 
-```</t>
+          <t>You are invited to the Annual Gala on July 20th at the Grand Ballroom, featuring dinner, entertainment, and an auction to support charitable initiatives. RSVP by July 10th.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>```
-Está invitado a la Gala Anual el 20 de julio a las 7:00 PM con cena, entretenimiento y una subasta. Confirme su asistencia antes del 10 de julio.
-```</t>
+          <t>Estás invitado a la Gala Anual el 20 de julio en el Gran Salón de Baile, que incluirá cena, entretenimiento y una subasta para apoyar iniciativas benéficas. Confirma tu asistencia antes del 10 de julio.</t>
         </is>
       </c>
     </row>
@@ -764,14 +748,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>```
-Niraj Wadhe wants to connect with Tejas to discuss potential collaboration opportunities, citing Tejas' insightful article on industry trends and a shared understanding of market dynamics. 
-```</t>
+          <t>Niraj Wadhe admires Tejas' article on industry trends and seeks collaboration, proposing a call next week to explore potential partnerships leveraging Tejas' expertise.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Niraj Wadhe desea conectarse con Tejas para discutir posibles oportunidades de colaboración, citando el artículo perspicaz de Tejas sobre las tendencias de la industria y una comprensión compartida de la dinámica del mercado.</t>
+          <t>Niraj Wadhe admira el artículo de Tejas sobre las tendencias de la industria y busca colaborar, proponiendo una llamada la próxima semana para explorar posibles asociaciones aprovechando la experiencia de Tejas.</t>
         </is>
       </c>
     </row>
@@ -802,14 +784,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>```
-This email reminds the patient of their appointment with Dr. Smith on June 30th at 10:00 AM and provides instructions for rescheduling or asking questions. 
-```</t>
+          <t>This email reminds you of your appointment with Dr. Smith on June 30th at 10:00 AM. Please arrive 10 minutes early and bring medical records. Contact the office if you need to reschedule or have questions.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Este correo electrónico le recuerda al paciente su cita con el Dr. Smith el 30 de junio a las 10:00 AM e incluye instrucciones para reprogramar o hacer preguntas.</t>
+          <t>Este correo electrónico es para recordarte tu cita con el Dr. Smith el 30 de junio a las 10:00 AM. Por favor, llega 10 minutos antes y trae tus registros médicos. Contacta a la oficina si necesitas reprogramar la cita o tienes alguna pregunta.</t>
         </is>
       </c>
     </row>
@@ -840,16 +820,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>```
-This June newsletter highlights new product launches, exclusive offers, and insightful articles. Click the provided link to access special discounts and learn more about upcoming products. 
-```</t>
+          <t>This June newsletter highlights new products, special discounts, and expert articles. Click the link to explore exclusive offers and stay updated on future innovations.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>```
-Este boletín de junio destaca nuevos lanzamientos de productos, ofertas exclusivas y artículos perspicaces. Haz clic en el enlace proporcionado para acceder a descuentos especiales y obtener más información sobre los próximos productos. 
-```</t>
+          <t>Este boletín de junio destaca nuevos productos, descuentos especiales y artículos de expertos. Haga clic en el enlace para explorar ofertas exclusivas y mantenerse actualizado sobre futuras innovaciones.</t>
         </is>
       </c>
     </row>

</xml_diff>